<commit_message>
Adds supplementary data query
Adds a query to retrieve data from ACL_SIGUMGO_SLV.
Also adds SUNAPIL to the ORDER BY clause of the initial query for more precise sorting.
</commit_message>
<xml_diff>
--- a/세입조정_이월_20251113.xlsx
+++ b/세입조정_이월_20251113.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\sidogeumgo_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D35379A-3A41-4050-ADD8-11AC99ACB3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69C75B3-F455-4104-AC2B-9EBF76A0D1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="67">
   <si>
     <t>KEORAEIL</t>
   </si>
@@ -106,9 +119,6 @@
     <t>103000</t>
   </si>
   <si>
-    <t>50000000000</t>
-  </si>
-  <si>
     <t>2024년회계 가이월/회계담당관34232</t>
   </si>
   <si>
@@ -118,9 +128,6 @@
     <t>20250109</t>
   </si>
   <si>
-    <t>100000000000</t>
-  </si>
-  <si>
     <t>2024년회계 가이월/회계담당관737</t>
   </si>
   <si>
@@ -130,9 +137,6 @@
     <t>20250110</t>
   </si>
   <si>
-    <t>150000000000</t>
-  </si>
-  <si>
     <t>2024년회계 가이월/회계담당관1030</t>
   </si>
   <si>
@@ -148,9 +152,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>21546163530</t>
-  </si>
-  <si>
     <t>2024년회계 최종이월/회계담당관2065</t>
   </si>
   <si>
@@ -163,9 +164,6 @@
     <t>209332</t>
   </si>
   <si>
-    <t>20000000000</t>
-  </si>
-  <si>
     <t>하수과-2/2025회계 가이월</t>
   </si>
   <si>
@@ -175,18 +173,12 @@
     <t>20250107</t>
   </si>
   <si>
-    <t>10000000000</t>
-  </si>
-  <si>
     <t>하수과-298/2025회계 가이월</t>
   </si>
   <si>
     <t>20250131</t>
   </si>
   <si>
-    <t>19073270454</t>
-  </si>
-  <si>
     <t>하수과-1182/2025회계 최종이월</t>
   </si>
   <si>
@@ -205,9 +197,6 @@
     <t>212400</t>
   </si>
   <si>
-    <t>10396915350</t>
-  </si>
-  <si>
     <t>지역개발기금/24&amp;gt;25회계이월</t>
   </si>
   <si>
@@ -223,9 +212,6 @@
     <t>212300</t>
   </si>
   <si>
-    <t>576299139898</t>
-  </si>
-  <si>
     <t>2024년회계이월/운영지원과902</t>
   </si>
   <si>
@@ -241,19 +227,23 @@
     <t>209330</t>
   </si>
   <si>
-    <t>136706926960</t>
-  </si>
-  <si>
     <t>경영관리부-5409/2025회계이월</t>
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>일반회계</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="#,##0_ "/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -329,7 +319,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -338,6 +328,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -673,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -695,7 +691,7 @@
     <col min="12" max="12" width="14.75" customWidth="1"/>
     <col min="13" max="13" width="14.875" customWidth="1"/>
     <col min="14" max="14" width="12.125" customWidth="1"/>
-    <col min="15" max="15" width="13.75" customWidth="1"/>
+    <col min="15" max="15" width="22.875" customWidth="1"/>
     <col min="16" max="16" width="12.375" customWidth="1"/>
     <col min="17" max="17" width="12.5" customWidth="1"/>
     <col min="18" max="18" width="58.5" customWidth="1"/>
@@ -797,39 +793,39 @@
       <c r="I2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -837,7 +833,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>23</v>
@@ -860,39 +856,39 @@
       <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>23</v>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3">
+        <v>100000000000</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -900,7 +896,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
@@ -923,39 +919,39 @@
       <c r="I4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>23</v>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>150000000000</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -963,7 +959,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -986,39 +982,39 @@
       <c r="I5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>23</v>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>100000000000</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="S5" s="2"/>
       <c r="T5" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -1049,44 +1045,44 @@
       <c r="I6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="2" t="s">
-        <v>23</v>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>21546163530</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S6" s="2"/>
       <c r="T6" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
@@ -1110,49 +1106,49 @@
         <v>25</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>20000000000</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -1173,49 +1169,49 @@
         <v>25</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>10000000000</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
@@ -1236,49 +1232,49 @@
         <v>25</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q9" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>19073270454</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="S9" s="2"/>
       <c r="T9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>23</v>
@@ -1299,46 +1295,46 @@
         <v>25</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
+        <v>10000000000</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>22</v>
@@ -1362,52 +1358,52 @@
         <v>25</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>23</v>
+        <v>53</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <v>10396915350</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>24</v>
@@ -1425,52 +1421,52 @@
         <v>25</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>23</v>
+        <v>58</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>576299139898</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="S12" s="2"/>
       <c r="T12" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>24</v>
@@ -1488,41 +1484,66 @@
         <v>25</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>23</v>
+        <v>63</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>136706926960</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="M14" s="4"/>
+      <c r="O14" s="4">
+        <f>SUM(O2:O13)</f>
+        <v>421546163530</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>103000</v>
+      </c>
+      <c r="J16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>209332</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>212400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds queries for analyzing carry-over amounts
Adds SQL queries to analyze carry-over amounts in the 세입월계표 (monthly revenue statement), focusing on itemized breakdowns (public funds deposit, time deposit) and accounting types (99, YY).

Includes queries targeting the RPT_DANGSEIPJOJEONG and ACL_SIGUMGO_SLV tables, filtering by date ranges, 금고 (treasury) codes, and comment contents.

Also adds Excel files related to the analysis.
</commit_message>
<xml_diff>
--- a/세입조정_이월_20251113.xlsx
+++ b/세입조정_이월_20251113.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\sidogeumgo_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69C75B3-F455-4104-AC2B-9EBF76A0D1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531227E7-9B50-42EB-9281-8879E0B3D8AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -272,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,6 +287,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -319,7 +325,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -335,9 +341,18 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -353,7 +368,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -672,7 +687,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1458,66 +1473,66 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="E13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="G13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0</v>
-      </c>
-      <c r="L13" s="3">
-        <v>0</v>
-      </c>
-      <c r="M13" s="3">
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
+        <v>0</v>
+      </c>
+      <c r="M13" s="6">
         <v>136706926960</v>
       </c>
-      <c r="N13" s="3">
-        <v>0</v>
-      </c>
-      <c r="O13" s="3">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>0</v>
-      </c>
-      <c r="R13" s="2" t="s">
+      <c r="N13" s="6">
+        <v>0</v>
+      </c>
+      <c r="O13" s="6">
+        <v>0</v>
+      </c>
+      <c r="P13" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>0</v>
+      </c>
+      <c r="R13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2" t="s">
+      <c r="S13" s="5"/>
+      <c r="T13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="U13" s="5" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>